<commit_message>
New version with bucle
This version have a bucle, but need fix some mistakes when search the values in the tables
</commit_message>
<xml_diff>
--- a/input_pdf_here/output.xlsx
+++ b/input_pdf_here/output.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\amazonTextractTables\input_pdf_here\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C815365-611F-41C2-BF48-B622B48DA523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>ts</t>
   </si>
@@ -242,13 +248,37 @@
   </si>
   <si>
     <t>38.12 0.11</t>
+  </si>
+  <si>
+    <t>40.5 + 4.1a</t>
+  </si>
+  <si>
+    <t>41.7 + 4.4a</t>
+  </si>
+  <si>
+    <t>45.3 + 4.8b</t>
+  </si>
+  <si>
+    <t>47.8 + 3.8b</t>
+  </si>
+  <si>
+    <t>61.3 + 2.8a</t>
+  </si>
+  <si>
+    <t>64.9 + 2.8bc</t>
+  </si>
+  <si>
+    <t>65.5 1.9°</t>
+  </si>
+  <si>
+    <t>63.3 + 1.0b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,11 +341,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -357,7 +395,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -389,9 +427,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -423,6 +479,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -598,14 +672,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,7 +727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -665,8 +749,14 @@
       <c r="G2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -688,8 +778,14 @@
       <c r="G3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="H3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -711,8 +807,14 @@
       <c r="G4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="H4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -734,8 +836,14 @@
       <c r="G5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="H5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -758,7 +866,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -781,7 +889,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -804,7 +912,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -827,7 +935,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -850,7 +958,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
         <v>75</v>
       </c>

</xml_diff>